<commit_message>
Update predictions and code
</commit_message>
<xml_diff>
--- a/predictions_2025-01-02.xlsx
+++ b/predictions_2025-01-02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -588,48 +588,48 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sc0</t>
+          <t>e3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Aberdeen</t>
+          <t>Gillingham</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ross County</t>
+          <t>Bromley</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1532.80060495642</v>
+        <v>1480.630280430628</v>
       </c>
       <c r="F2" t="n">
-        <v>1446.848010478442</v>
+        <v>1532.144152754764</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1.96</t>
+          <t>6.02</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>4.47</t>
+          <t>4.10</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3.99</t>
+          <t>1.72</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1.74</t>
+          <t>2.52</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2.35</t>
+          <t>1.66</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -639,27 +639,27 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>1.61</t>
+          <t>3.07</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>5.03</t>
+          <t>3.16</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>5.59</t>
+          <t>2.79</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1.48</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>3.09</t>
+          <t>1.80</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -669,27 +669,27 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>1.59</t>
+          <t>2.80</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>5.24</t>
+          <t>3.74</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>5.52</t>
+          <t>2.67</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>1.46</t>
+          <t>2.23</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>3.18</t>
+          <t>1.81</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
@@ -699,27 +699,27 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>7.45</t>
+          <t>5.51</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.31</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>25.84</t>
+          <t>18.19</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>7.69</t>
+          <t>6.07</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>1.15</t>
+          <t>1.20</t>
         </is>
       </c>
     </row>
@@ -731,48 +731,48 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sc0</t>
+          <t>e3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hearts</t>
+          <t>Newport County</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Motherwell</t>
+          <t>AFC Wimbledon</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1438.753674504617</v>
+        <v>1474.753588871106</v>
       </c>
       <c r="F3" t="n">
-        <v>1497.172023959643</v>
+        <v>1539.074720758685</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.69</t>
+          <t>7.78</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>4.10</t>
+          <t>5.19</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2.67</t>
+          <t>1.53</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1.84</t>
+          <t>1.88</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>2.13</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -782,27 +782,27 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2.04</t>
+          <t>3.59</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>4.42</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>3.51</t>
+          <t>2.12</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>1.56</t>
+          <t>1.70</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>2.77</t>
+          <t>2.44</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -812,27 +812,27 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>2.01</t>
+          <t>3.41</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>4.43</t>
+          <t>4.34</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>3.60</t>
+          <t>2.10</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>1.54</t>
+          <t>1.65</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>2.85</t>
+          <t>2.53</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
@@ -842,27 +842,27 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>49.55</t>
+          <t>3.99</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>1.06</t>
+          <t>1.73</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>25.78</t>
+          <t>5.80</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>28.45</t>
+          <t>1.16</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>1.04</t>
+          <t>7.42</t>
         </is>
       </c>
     </row>
@@ -879,43 +879,43 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Kilmarnock</t>
+          <t>Aberdeen</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>St Mirren</t>
+          <t>Ross County</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1482.386000125386</v>
+        <v>1532.80060495642</v>
       </c>
       <c r="F4" t="n">
-        <v>1512.632322257115</v>
+        <v>1446.848010478442</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4.35</t>
+          <t>1.96</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>4.22</t>
+          <t>4.47</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.91</t>
+          <t>3.99</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2.19</t>
+          <t>1.74</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>1.84</t>
+          <t>2.35</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -925,27 +925,27 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2.44</t>
+          <t>1.39</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>3.98</t>
+          <t>6.61</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2.96</t>
+          <t>7.85</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>1.76</t>
+          <t>1.32</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>2.32</t>
+          <t>4.14</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -955,27 +955,27 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2.41</t>
+          <t>1.40</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>4.08</t>
+          <t>6.60</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>2.94</t>
+          <t>7.34</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>1.73</t>
+          <t>1.30</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>2.37</t>
+          <t>4.30</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -985,27 +985,27 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>3.48</t>
+          <t>8.47</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>1.62</t>
+          <t>1.21</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>10.34</t>
+          <t>19.06</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>1.80</t>
+          <t>13.88</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>2.24</t>
+          <t>1.08</t>
         </is>
       </c>
     </row>
@@ -1022,43 +1022,43 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rangers</t>
+          <t>Hearts</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Celtic</t>
+          <t>Motherwell</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1570.310970943068</v>
+        <v>1438.753674504617</v>
       </c>
       <c r="F5" t="n">
-        <v>1657.782096290991</v>
+        <v>1497.172023959643</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>16.42</t>
+          <t>2.69</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3.30</t>
+          <t>4.10</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1.58</t>
+          <t>2.67</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>5.56</t>
+          <t>1.84</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>1.22</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -1068,27 +1068,27 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>4.32</t>
+          <t>1.85</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2.92</t>
+          <t>4.73</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2.35</t>
+          <t>4.04</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>3.54</t>
+          <t>1.46</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>1.39</t>
+          <t>3.19</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1098,27 +1098,27 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
+          <t>1.87</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>4.75</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
           <t>3.91</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>3.17</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>2.33</t>
-        </is>
-      </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>3.56</t>
+          <t>1.44</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>1.39</t>
+          <t>3.27</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
@@ -1128,27 +1128,27 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>2.77</t>
+          <t>11.57</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>4.43</t>
+          <t>1.18</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>2.42</t>
+          <t>14.69</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>3.59</t>
+          <t>24.28</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>1.39</t>
+          <t>1.04</t>
         </is>
       </c>
     </row>
@@ -1165,43 +1165,43 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>St Johnstone</t>
+          <t>Kilmarnock</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hibernian</t>
+          <t>St Mirren</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>1400.418251343876</v>
+        <v>1482.386000125386</v>
       </c>
       <c r="F6" t="n">
-        <v>1491.062685329437</v>
+        <v>1512.632322257115</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>6.46</t>
+          <t>4.35</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>5.62</t>
+          <t>4.22</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1.60</t>
+          <t>1.91</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1.55</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2.81</t>
+          <t>1.84</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -1211,27 +1211,27 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2.48</t>
+          <t>2.19</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>4.49</t>
+          <t>4.14</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>2.68</t>
+          <t>3.32</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>1.42</t>
+          <t>1.68</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>3.39</t>
+          <t>2.47</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1241,27 +1241,27 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>2.44</t>
+          <t>2.20</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>4.73</t>
+          <t>4.20</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>2.63</t>
+          <t>3.26</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>1.38</t>
+          <t>1.64</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>3.66</t>
+          <t>2.55</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
@@ -1271,27 +1271,27 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>8.11</t>
+          <t>7.38</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>8.75</t>
+          <t>1.34</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>1.31</t>
+          <t>8.47</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>1.07</t>
+          <t>1.33</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>14.87</t>
+          <t>4.06</t>
         </is>
       </c>
     </row>
@@ -1308,133 +1308,419 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Rangers</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Celtic</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1570.310970943068</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1657.782096290991</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>16.42</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>3.30</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>5.56</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Bivariantní Poisson</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>2.44</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>3.40</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>3.38</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>2.36</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Monte Carlo</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>2.38</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>3.67</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>3.25</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>xGBoost</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>2.22</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>6.67</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>2.50</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>3.26</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Základní Poisson</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>sc0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>St Johnstone</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Hibernian</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1400.418251343876</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1491.062685329437</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>6.46</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>5.62</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1.60</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2.81</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Bivariantní Poisson</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>4.61</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>2.83</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>1.36</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>3.79</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Monte Carlo</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>4.96</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>2.82</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>3.93</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>xGBoost</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>7.32</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>6.00</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>1.07</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>15.42</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Základní Poisson</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sc0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Dundee</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Dundee United</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E9" t="n">
         <v>1451.255965411684</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F9" t="n">
         <v>1529.921564811205</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>5.27</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>5.59</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>1.69</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>1.55</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>2.83</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Bivariantní Poisson</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>2.82</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>4.59</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2.34</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>1.34</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>3.92</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2.38</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>4.79</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>4.42</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
         <is>
           <t>Monte Carlo</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>2.72</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>4.89</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>2.34</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>1.33</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>4.03</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>4.97</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>2.63</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>4.85</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
         <is>
           <t>xGBoost</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>8.01</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>1.20</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>22.31</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>1.54</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>2.85</t>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>7.10</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>23.64</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>4.44</t>
         </is>
       </c>
     </row>

</xml_diff>